<commit_message>
Added items and characters
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corn/Library/Mobile Documents/com~apple~CloudDocs/University/Year1/Q1/Programming/CBL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corn/Documents/TheHolyBier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19390B73-6821-A44C-9783-264BDBE6158B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B0F804-B6BF-F544-9F8C-E696DEC6D7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="2100" windowWidth="34840" windowHeight="20860" xr2:uid="{05F98CA3-5506-3D41-AB8B-B8E2066328B9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{05F98CA3-5506-3D41-AB8B-B8E2066328B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -77,9 +77,6 @@
     <t xml:space="preserve">A path can be one of the following: field boss fight, a room (with an item), or main boss fight. </t>
   </si>
   <si>
-    <t xml:space="preserve">If the character is on a room (with an item), he can chose to switch one of his/her items to another. </t>
-  </si>
-  <si>
     <t>Yes / No appears, if Yes pressed, a certain item in the inventory changes.</t>
   </si>
   <si>
@@ -111,6 +108,15 @@
   </si>
   <si>
     <t>Pressing the inventory button lists all the items that we own.</t>
+  </si>
+  <si>
+    <t>Accessing stats menu</t>
+  </si>
+  <si>
+    <t>Open the path chose screen, and you can see the player stats on the bottom left.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the character is in a room (with an item), he can chose one of the buttons to switch one of his/her items to another. </t>
   </si>
 </sst>
 </file>
@@ -649,7 +655,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="70.83203125" defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -667,7 +673,7 @@
     </row>
     <row r="2" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -684,7 +690,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -712,46 +718,50 @@
         <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>